<commit_message>
Added Total Clan Stars
</commit_message>
<xml_diff>
--- a/charts/war20240914.xlsx
+++ b/charts/war20240914.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,6 +486,11 @@
           <t>Total Stars</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Total Clan Stars</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -514,6 +519,9 @@
       <c r="H2" s="2" t="n">
         <v>6</v>
       </c>
+      <c r="I2" s="2" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -542,6 +550,9 @@
       <c r="H3" s="2" t="n">
         <v>6</v>
       </c>
+      <c r="I3" s="2" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -570,6 +581,9 @@
       <c r="H4" s="2" t="n">
         <v>6</v>
       </c>
+      <c r="I4" s="2" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -598,6 +612,9 @@
       <c r="H5" s="2" t="n">
         <v>5</v>
       </c>
+      <c r="I5" s="2" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -626,6 +643,9 @@
       <c r="H6" s="2" t="n">
         <v>4</v>
       </c>
+      <c r="I6" s="2" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -654,6 +674,9 @@
       <c r="H7" s="2" t="n">
         <v>4</v>
       </c>
+      <c r="I7" s="2" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -682,6 +705,9 @@
       <c r="H8" s="2" t="n">
         <v>3</v>
       </c>
+      <c r="I8" s="2" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -710,6 +736,9 @@
       <c r="H9" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="I9" s="3" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -738,6 +767,9 @@
       <c r="H10" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="I10" s="3" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -766,6 +798,9 @@
       <c r="H11" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="I11" s="3" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -794,6 +829,9 @@
       <c r="H12" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="I12" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -822,6 +860,9 @@
       <c r="H13" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="I13" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -850,6 +891,9 @@
       <c r="H14" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="I14" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -878,6 +922,9 @@
       <c r="H15" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="I15" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -904,6 +951,9 @@
         <v>0</v>
       </c>
       <c r="H16" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>